<commit_message>
Does not check dates for the collection records
</commit_message>
<xml_diff>
--- a/herbarium label_HU/herbarium_specimens_label_data.xlsx
+++ b/herbarium label_HU/herbarium_specimens_label_data.xlsx
@@ -77,48 +77,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Please check the date</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G19" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Please check the date</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AJ19" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Please check the date</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>GLOBAL_UNIQUE_IDENTIFIER</t>
   </si>
@@ -358,6 +322,9 @@
   </si>
   <si>
     <t>2014-01-18</t>
+  </si>
+  <si>
+    <t>2016 nian 01 yue 18 ri</t>
   </si>
   <si>
     <t>短花梗黃耆</t>
@@ -1512,7 +1479,7 @@
       <c r="F8" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" t="s">
         <v>71</v>
       </c>
       <c r="H8" t="s">
@@ -1913,7 +1880,7 @@
         <v>43</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="H12" t="s">
         <v>45</v>
@@ -2016,19 +1983,19 @@
         <v>65</v>
       </c>
       <c r="H13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M13" t="s">
         <v>50</v>
@@ -2212,19 +2179,19 @@
         <v>65</v>
       </c>
       <c r="H15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M15" t="s">
         <v>50</v>
@@ -2310,19 +2277,19 @@
         <v>65</v>
       </c>
       <c r="H16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K16" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="L16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M16" t="s">
         <v>50</v>
@@ -2604,23 +2571,23 @@
       <c r="F19" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>94</v>
+      <c r="G19" t="s">
+        <v>95</v>
       </c>
       <c r="H19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M19" t="s">
         <v>50</v>
@@ -2681,8 +2648,8 @@
       <c r="AI19" t="s">
         <v>42</v>
       </c>
-      <c r="AJ19" s="1" t="s">
-        <v>100</v>
+      <c r="AJ19" t="s">
+        <v>101</v>
       </c>
       <c r="AK19"/>
       <c r="AL19"/>

</xml_diff>